<commit_message>
Pegando a tividade do OverFlow para resolver
</commit_message>
<xml_diff>
--- a/controle.xlsx
+++ b/controle.xlsx
@@ -301,7 +301,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,8 +337,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,6 +360,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -380,12 +392,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -408,8 +421,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Bom" xfId="3" builtinId="26"/>
     <cellStyle name="Célula de Verificação" xfId="2" builtinId="23"/>
     <cellStyle name="Incorreto" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,7 +739,7 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,11 +984,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
         <v>42165</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -974,8 +998,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="7" t="s">
@@ -985,8 +1010,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -996,8 +1022,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="7" t="s">
@@ -1007,8 +1034,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="7" t="s">
@@ -1285,13 +1313,16 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="A42" s="9">
+        <v>42203</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1478,11 +1509,6 @@
       <filters>
         <filter val="Aguardando"/>
         <filter val="Em Andamento"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Codificação"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Pegando o Create para trata
</commit_message>
<xml_diff>
--- a/controle.xlsx
+++ b/controle.xlsx
@@ -739,7 +739,7 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,13 +1349,16 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="A45" s="9">
+        <v>42203</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizando o controle de atvs
</commit_message>
<xml_diff>
--- a/controle.xlsx
+++ b/controle.xlsx
@@ -721,7 +721,7 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1300,7 +1300,7 @@
         <v>42203</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>0</v>
@@ -1350,7 +1350,7 @@
         <v>42203</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Incluindo algumas práticas de otimização em Js
</commit_message>
<xml_diff>
--- a/controle.xlsx
+++ b/controle.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tarefas" sheetId="1" r:id="rId1"/>
     <sheet name="Anotações Gerais" sheetId="2" r:id="rId2"/>
     <sheet name="Depois da qualificacao" sheetId="3" r:id="rId3"/>
+    <sheet name="mutações" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tarefas!$A$1:$D$57</definedName>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="94">
   <si>
     <t>Codificação</t>
   </si>
@@ -295,6 +296,51 @@
   </si>
   <si>
     <t>Colocar um report de saída em HTML com o diff dos arquivos (Best x original) Ver script pronto (http://ejohn.org/projects/javascript-diff-algorithm/)</t>
+  </si>
+  <si>
+    <t>Fazer a otimização sequencial das funções?</t>
+  </si>
+  <si>
+    <t>Retirar globais</t>
+  </si>
+  <si>
+    <t>Retirar var de dentro de for</t>
+  </si>
+  <si>
+    <t>http://pt.slideshare.net/doris1/performance-optimization-and-javascript-best-practices</t>
+  </si>
+  <si>
+    <t>http://jonraasch.com/blog/10-javascript-performance-boosting-tips-from-nicholas-zakas</t>
+  </si>
+  <si>
+    <t>Apagar instruções com with()</t>
+  </si>
+  <si>
+    <t>Trocar for in por for puro</t>
+  </si>
+  <si>
+    <t>Trocar for por while com variavel de controle externa (item 7)</t>
+  </si>
+  <si>
+    <t>Use === Instead of ==</t>
+  </si>
+  <si>
+    <t>http://blogs.msdn.com/b/dorischen/archive/2011/03/17/web-performance-tips-10-javascript-best-practices.aspx</t>
+  </si>
+  <si>
+    <t>Eval = Bad</t>
+  </si>
+  <si>
+    <t>Reduce Globals: Namespace</t>
+  </si>
+  <si>
+    <t>Don't Pass a String to "SetInterval" or "SetTimeOut"</t>
+  </si>
+  <si>
+    <t>Use {} Instead of New Object()</t>
+  </si>
+  <si>
+    <t>Use [] Instead of New Array()</t>
   </si>
 </sst>
 </file>
@@ -338,7 +384,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,6 +399,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -385,7 +437,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -414,6 +466,7 @@
     <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Célula de Verificação" xfId="2" builtinId="23"/>
@@ -720,8 +773,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B58" sqref="B58:D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,8 +1535,11 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>42204</v>
+      </c>
       <c r="B57" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>0</v>
@@ -1511,7 +1567,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,6 +1594,11 @@
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
@@ -1614,4 +1675,86 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="81.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="104.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Nova Ref do Jurassic
</commit_message>
<xml_diff>
--- a/controle.xlsx
+++ b/controle.xlsx
@@ -774,7 +774,7 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1351,7 +1351,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>42203</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>42203</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>42203</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>42204</v>
       </c>

</xml_diff>

<commit_message>
Bug na validação do OverFlow em javascript
</commit_message>
<xml_diff>
--- a/controle.xlsx
+++ b/controle.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="95">
   <si>
     <t>Codificação</t>
   </si>
@@ -341,6 +341,9 @@
   </si>
   <si>
     <t>Use [] Instead of New Array()</t>
+  </si>
+  <si>
+    <t>OverFlow no javascript, refatoração do Jurassic</t>
   </si>
 </sst>
 </file>
@@ -771,10 +774,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1549,6 +1552,20 @@
       </c>
       <c r="D57" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>42205</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tentando tratar o terceiro tipo de overflow
</commit_message>
<xml_diff>
--- a/controle.xlsx
+++ b/controle.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="96">
   <si>
     <t>Codificação</t>
   </si>
@@ -344,6 +344,9 @@
   </si>
   <si>
     <t>OverFlow no javascript, refatoração do Jurassic</t>
+  </si>
+  <si>
+    <t>OverFlow quando usa a função Clone</t>
   </si>
 </sst>
 </file>
@@ -774,10 +777,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,6 +1569,20 @@
       </c>
       <c r="D58" s="3" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>42206</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Atualização do controle"
This reverts commit 2ecc3a388c05840f526286ffe7108a33a0a6e3ab.
</commit_message>
<xml_diff>
--- a/controle.xlsx
+++ b/controle.xlsx
@@ -13,7 +13,7 @@
     <sheet name="mutações" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tarefas!$A$1:$D$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tarefas!$A$1:$D$57</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
@@ -54,36 +54,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B59" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Autor:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Concluída em 28/07/2015</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="96">
   <si>
     <t>Codificação</t>
   </si>
@@ -136,6 +112,9 @@
     <t>Mudar o parser para criar um individuo em cima da AST que o ANTLR gera</t>
   </si>
   <si>
+    <t>Executar as rodadas</t>
+  </si>
+  <si>
     <t>Concluída</t>
   </si>
   <si>
@@ -368,22 +347,13 @@
   </si>
   <si>
     <t>OverFlow quando usa a função Clone</t>
-  </si>
-  <si>
-    <t>Incluir a underscore na execução</t>
-  </si>
-  <si>
-    <t>Executar as rodadas da momentJs</t>
-  </si>
-  <si>
-    <t>Executar as rodadas do underscore</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,19 +388,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -820,10 +777,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +793,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -845,7 +802,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -853,7 +810,7 @@
         <v>42165</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
@@ -867,7 +824,7 @@
         <v>42167</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -881,7 +838,7 @@
         <v>42167</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
@@ -895,7 +852,7 @@
         <v>42167</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>0</v>
@@ -909,7 +866,7 @@
         <v>42168</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>0</v>
@@ -923,13 +880,13 @@
         <v>42168</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -937,7 +894,7 @@
         <v>42168</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>0</v>
@@ -951,7 +908,7 @@
         <v>42173</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>0</v>
@@ -965,7 +922,7 @@
         <v>42173</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>0</v>
@@ -979,7 +936,7 @@
         <v>42175</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>0</v>
@@ -993,7 +950,7 @@
         <v>42175</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>0</v>
@@ -1007,7 +964,7 @@
         <v>42175</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>0</v>
@@ -1021,7 +978,7 @@
         <v>42175</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>0</v>
@@ -1035,7 +992,7 @@
         <v>42175</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>0</v>
@@ -1049,7 +1006,7 @@
         <v>42179</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>0</v>
@@ -1058,80 +1015,80 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>42204</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>42165</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1139,13 +1096,13 @@
         <v>42181</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1153,13 +1110,13 @@
         <v>42190</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1167,13 +1124,13 @@
         <v>42190</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1181,13 +1138,13 @@
         <v>42190</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1195,13 +1152,13 @@
         <v>42190</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1209,13 +1166,13 @@
         <v>42190</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1223,13 +1180,13 @@
         <v>42190</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1237,13 +1194,13 @@
         <v>42190</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1251,13 +1208,13 @@
         <v>42196</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1265,13 +1222,13 @@
         <v>42196</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1279,13 +1236,13 @@
         <v>42196</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1293,13 +1250,13 @@
         <v>42196</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1307,13 +1264,13 @@
         <v>42196</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1321,13 +1278,13 @@
         <v>42197</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1335,13 +1292,13 @@
         <v>42197</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1349,13 +1306,13 @@
         <v>42197</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1363,13 +1320,13 @@
         <v>42197</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1377,13 +1334,13 @@
         <v>42197</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1391,13 +1348,13 @@
         <v>42197</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1405,35 +1362,35 @@
         <v>42203</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1441,13 +1398,13 @@
         <v>42203</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1455,79 +1412,79 @@
         <v>42203</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D48" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1535,13 +1492,13 @@
         <v>42199</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1549,13 +1506,13 @@
         <v>42199</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1563,13 +1520,13 @@
         <v>42200</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1577,13 +1534,13 @@
         <v>42200</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1591,70 +1548,45 @@
         <v>42204</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>42205</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>42206</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
-        <v>42221</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D60" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D60">
+  <autoFilter ref="A1:D57">
     <filterColumn colId="1">
       <filters>
         <filter val="Aguardando"/>
@@ -1683,42 +1615,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1741,40 +1673,40 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1799,64 +1731,64 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Atualização do controle""
This reverts commit bff6ec14c480ee83503b8b45911e4bea6d9da5c4.
</commit_message>
<xml_diff>
--- a/controle.xlsx
+++ b/controle.xlsx
@@ -13,7 +13,7 @@
     <sheet name="mutações" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tarefas!$A$1:$D$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tarefas!$A$1:$D$60</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
@@ -54,12 +54,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="B59" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Autor:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Concluída em 28/07/2015</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="98">
   <si>
     <t>Codificação</t>
   </si>
@@ -112,9 +136,6 @@
     <t>Mudar o parser para criar um individuo em cima da AST que o ANTLR gera</t>
   </si>
   <si>
-    <t>Executar as rodadas</t>
-  </si>
-  <si>
     <t>Concluída</t>
   </si>
   <si>
@@ -347,13 +368,22 @@
   </si>
   <si>
     <t>OverFlow quando usa a função Clone</t>
+  </si>
+  <si>
+    <t>Incluir a underscore na execução</t>
+  </si>
+  <si>
+    <t>Executar as rodadas da momentJs</t>
+  </si>
+  <si>
+    <t>Executar as rodadas do underscore</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,6 +418,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -777,10 +820,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,7 +836,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -802,7 +845,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -810,7 +853,7 @@
         <v>42165</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
@@ -824,7 +867,7 @@
         <v>42167</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -838,7 +881,7 @@
         <v>42167</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
@@ -852,7 +895,7 @@
         <v>42167</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>0</v>
@@ -866,7 +909,7 @@
         <v>42168</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>0</v>
@@ -880,13 +923,13 @@
         <v>42168</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -894,7 +937,7 @@
         <v>42168</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>0</v>
@@ -908,7 +951,7 @@
         <v>42173</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>0</v>
@@ -922,7 +965,7 @@
         <v>42173</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>0</v>
@@ -936,7 +979,7 @@
         <v>42175</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>0</v>
@@ -950,7 +993,7 @@
         <v>42175</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>0</v>
@@ -964,7 +1007,7 @@
         <v>42175</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>0</v>
@@ -978,7 +1021,7 @@
         <v>42175</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>0</v>
@@ -992,7 +1035,7 @@
         <v>42175</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>0</v>
@@ -1006,7 +1049,7 @@
         <v>42179</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>0</v>
@@ -1015,80 +1058,80 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>42204</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>42165</v>
       </c>
       <c r="B18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1096,13 +1139,13 @@
         <v>42181</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1110,13 +1153,13 @@
         <v>42190</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1124,13 +1167,13 @@
         <v>42190</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1138,13 +1181,13 @@
         <v>42190</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1152,13 +1195,13 @@
         <v>42190</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1166,13 +1209,13 @@
         <v>42190</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1180,13 +1223,13 @@
         <v>42190</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1194,13 +1237,13 @@
         <v>42190</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1208,13 +1251,13 @@
         <v>42196</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1222,13 +1265,13 @@
         <v>42196</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1236,13 +1279,13 @@
         <v>42196</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1250,13 +1293,13 @@
         <v>42196</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1264,13 +1307,13 @@
         <v>42196</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1278,13 +1321,13 @@
         <v>42197</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1292,13 +1335,13 @@
         <v>42197</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1306,13 +1349,13 @@
         <v>42197</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1320,13 +1363,13 @@
         <v>42197</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1334,13 +1377,13 @@
         <v>42197</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1348,13 +1391,13 @@
         <v>42197</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1362,35 +1405,35 @@
         <v>42203</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1398,13 +1441,13 @@
         <v>42203</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1412,79 +1455,79 @@
         <v>42203</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1492,13 +1535,13 @@
         <v>42199</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1506,13 +1549,13 @@
         <v>42199</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1520,13 +1563,13 @@
         <v>42200</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1534,13 +1577,13 @@
         <v>42200</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -1548,45 +1591,70 @@
         <v>42204</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>42205</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>42206</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D59" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>42221</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>95</v>
       </c>
     </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D57">
+  <autoFilter ref="A1:D60">
     <filterColumn colId="1">
       <filters>
         <filter val="Aguardando"/>
@@ -1615,42 +1683,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1673,40 +1741,40 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
         <v>69</v>
-      </c>
-      <c r="B2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1731,64 +1799,64 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" t="s">
         <v>82</v>
       </c>
-      <c r="B1" t="s">
-        <v>83</v>
-      </c>
       <c r="C1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>